<commit_message>
Veracity performance testing. Realized that multinomial HMM implementation is faulty - Deprecated for now.
</commit_message>
<xml_diff>
--- a/src/performance_testing/dast_performance.xlsx
+++ b/src/performance_testing/dast_performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="length_dataset" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="20">
   <si>
     <t>model</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>10+</t>
+  </si>
+  <si>
+    <t>dast_majority</t>
+  </si>
+  <si>
+    <t>pheme_majority</t>
+  </si>
+  <si>
+    <t>dastpheme_majority</t>
   </si>
 </sst>
 </file>
@@ -984,11 +993,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="475999192"/>
-        <c:axId val="475998016"/>
+        <c:axId val="506690840"/>
+        <c:axId val="506680648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475999192"/>
+        <c:axId val="506690840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,7 +1040,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475998016"/>
+        <c:crossAx val="506680648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1039,7 +1048,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="475998016"/>
+        <c:axId val="506680648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +1099,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475999192"/>
+        <c:crossAx val="506690840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1542,11 +1551,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="551283520"/>
-        <c:axId val="551277640"/>
+        <c:axId val="506703384"/>
+        <c:axId val="506704168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551283520"/>
+        <c:axId val="506703384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1598,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551277640"/>
+        <c:crossAx val="506704168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1597,7 +1606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551277640"/>
+        <c:axId val="506704168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,7 +1657,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551283520"/>
+        <c:crossAx val="506703384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2100,11 +2109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="544362648"/>
-        <c:axId val="544359904"/>
+        <c:axId val="506701424"/>
+        <c:axId val="506696720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="544362648"/>
+        <c:axId val="506701424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,7 +2156,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="544359904"/>
+        <c:crossAx val="506696720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2155,7 +2164,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="544359904"/>
+        <c:axId val="506696720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2206,7 +2215,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="544362648"/>
+        <c:crossAx val="506701424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2660,11 +2669,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="475994488"/>
-        <c:axId val="475994880"/>
+        <c:axId val="506699464"/>
+        <c:axId val="506700248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475994488"/>
+        <c:axId val="506699464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2707,7 +2716,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475994880"/>
+        <c:crossAx val="506700248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2715,7 +2724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="475994880"/>
+        <c:axId val="506700248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,7 +2775,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475994488"/>
+        <c:crossAx val="506699464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3220,11 +3229,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="475996448"/>
-        <c:axId val="475996840"/>
+        <c:axId val="506694760"/>
+        <c:axId val="506701816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475996448"/>
+        <c:axId val="506694760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3267,7 +3276,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475996840"/>
+        <c:crossAx val="506701816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3275,7 +3284,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="475996840"/>
+        <c:axId val="506701816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3326,7 +3335,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475996448"/>
+        <c:crossAx val="506694760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3780,11 +3789,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="539104128"/>
-        <c:axId val="539104912"/>
+        <c:axId val="506702992"/>
+        <c:axId val="506693976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539104128"/>
+        <c:axId val="506702992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3827,7 +3836,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539104912"/>
+        <c:crossAx val="506693976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3835,7 +3844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539104912"/>
+        <c:axId val="506693976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3886,7 +3895,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539104128"/>
+        <c:crossAx val="506702992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4340,11 +4349,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="539107656"/>
-        <c:axId val="539107264"/>
+        <c:axId val="506700640"/>
+        <c:axId val="506694368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539107656"/>
+        <c:axId val="506700640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4387,7 +4396,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539107264"/>
+        <c:crossAx val="506694368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4395,7 +4404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539107264"/>
+        <c:axId val="506694368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4446,7 +4455,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539107656"/>
+        <c:crossAx val="506700640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4900,11 +4909,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="539106088"/>
-        <c:axId val="539108048"/>
+        <c:axId val="506701032"/>
+        <c:axId val="506696328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539106088"/>
+        <c:axId val="506701032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4947,7 +4956,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539108048"/>
+        <c:crossAx val="506696328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4955,7 +4964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539108048"/>
+        <c:axId val="506696328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5006,7 +5015,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539106088"/>
+        <c:crossAx val="506701032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5460,11 +5469,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="539103736"/>
-        <c:axId val="539104520"/>
+        <c:axId val="506698288"/>
+        <c:axId val="506697504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539103736"/>
+        <c:axId val="506698288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5507,7 +5516,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539104520"/>
+        <c:crossAx val="506697504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5515,7 +5524,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539104520"/>
+        <c:axId val="506697504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5566,7 +5575,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539103736"/>
+        <c:crossAx val="506698288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5673,7 +5682,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]dataset_splits!$B$1</c:f>
+              <c:f>dataset!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5753,53 +5762,71 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>[1]dataset_splits!$A$2:$A$7</c:f>
+              <c:f>dataset!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme</c:v>
+                <c:pt idx="6">
+                  <c:v>dast_majority</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>pheme_majority</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dastpheme_majority</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]dataset_splits!$B$2:$B$7</c:f>
+              <c:f>dataset!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.48</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.45</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.49</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.47</c:v>
+                <c:pt idx="6">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5810,7 +5837,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]dataset_splits!$C$1</c:f>
+              <c:f>dataset!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5890,53 +5917,71 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>[1]dataset_splits!$A$2:$A$7</c:f>
+              <c:f>dataset!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>dast_ts</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>pheme_ts</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dastpheme_ts</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>pheme</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dastpheme</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>dast</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>pheme</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>dastpheme</c:v>
+                <c:pt idx="6">
+                  <c:v>dast_majority</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>pheme_majority</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dastpheme_majority</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]dataset_splits!$C$2:$C$7</c:f>
+              <c:f>dataset!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.77</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.77</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76</c:v>
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5952,11 +5997,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="539106480"/>
-        <c:axId val="539108440"/>
+        <c:axId val="506711224"/>
+        <c:axId val="506710048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="539106480"/>
+        <c:axId val="506711224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5999,7 +6044,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539108440"/>
+        <c:crossAx val="506710048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6007,7 +6052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539108440"/>
+        <c:axId val="506710048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6058,7 +6103,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539106480"/>
+        <c:crossAx val="506711224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6500,11 +6545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="475998800"/>
-        <c:axId val="475995272"/>
+        <c:axId val="506681432"/>
+        <c:axId val="506680256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475998800"/>
+        <c:axId val="506681432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6547,7 +6592,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475995272"/>
+        <c:crossAx val="506680256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6555,7 +6600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="475995272"/>
+        <c:axId val="506680256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6606,7 +6651,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475998800"/>
+        <c:crossAx val="506681432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7048,11 +7093,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="475994096"/>
-        <c:axId val="475995664"/>
+        <c:axId val="506686528"/>
+        <c:axId val="506683000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475994096"/>
+        <c:axId val="506686528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7095,7 +7140,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475995664"/>
+        <c:crossAx val="506683000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7103,7 +7148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="475995664"/>
+        <c:axId val="506683000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7154,7 +7199,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475994096"/>
+        <c:crossAx val="506686528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7596,11 +7641,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="475999976"/>
-        <c:axId val="476000368"/>
+        <c:axId val="506683784"/>
+        <c:axId val="506688880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="475999976"/>
+        <c:axId val="506683784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7643,7 +7688,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="476000368"/>
+        <c:crossAx val="506688880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7651,7 +7696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="476000368"/>
+        <c:axId val="506688880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7702,7 +7747,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="475999976"/>
+        <c:crossAx val="506683784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8154,11 +8199,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="392909832"/>
-        <c:axId val="392911400"/>
+        <c:axId val="506686136"/>
+        <c:axId val="506687704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="392909832"/>
+        <c:axId val="506686136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8201,7 +8246,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392911400"/>
+        <c:crossAx val="506687704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8209,7 +8254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392911400"/>
+        <c:axId val="506687704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8260,7 +8305,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392909832"/>
+        <c:crossAx val="506686136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8712,11 +8757,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="551267056"/>
-        <c:axId val="551267448"/>
+        <c:axId val="506688096"/>
+        <c:axId val="506689664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551267056"/>
+        <c:axId val="506688096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8759,7 +8804,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551267448"/>
+        <c:crossAx val="506689664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8767,7 +8812,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551267448"/>
+        <c:axId val="506689664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8818,7 +8863,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551267056"/>
+        <c:crossAx val="506688096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9270,11 +9315,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="551285480"/>
-        <c:axId val="551290968"/>
+        <c:axId val="506691232"/>
+        <c:axId val="506698680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551285480"/>
+        <c:axId val="506691232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9317,7 +9362,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551290968"/>
+        <c:crossAx val="506698680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9325,7 +9370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551290968"/>
+        <c:axId val="506698680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9376,7 +9421,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551285480"/>
+        <c:crossAx val="506691232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9828,11 +9873,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="551277248"/>
-        <c:axId val="551280384"/>
+        <c:axId val="506697112"/>
+        <c:axId val="506699856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="551277248"/>
+        <c:axId val="506697112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9875,7 +9920,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551280384"/>
+        <c:crossAx val="506699856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9883,7 +9928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551280384"/>
+        <c:axId val="506699856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9934,7 +9979,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551277248"/>
+        <c:crossAx val="506697112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10386,11 +10431,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="549879856"/>
-        <c:axId val="549870840"/>
+        <c:axId val="506695544"/>
+        <c:axId val="506702600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="549879856"/>
+        <c:axId val="506695544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10433,7 +10478,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549870840"/>
+        <c:crossAx val="506702600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10441,7 +10486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="549870840"/>
+        <c:axId val="506702600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10492,7 +10537,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549879856"/>
+        <c:crossAx val="506695544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23209,8 +23254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23829,10 +23874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23850,10 +23895,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="C2">
         <v>0.77</v>
@@ -23861,57 +23906,90 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="C3">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.48</v>
       </c>
       <c r="C4">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>0.49</v>
+        <v>0.44</v>
       </c>
       <c r="C5">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="C6">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
       <c r="C7">
-        <v>0.76</v>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>0.44</v>
+      </c>
+      <c r="C8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>0.44</v>
+      </c>
+      <c r="C9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>0.44</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>